<commit_message>
Getoetst met catalogus versie 2.1; geen impact.
</commit_message>
<xml_diff>
--- a/INSPIRE/BHR-G INSPIRE mapping.xlsx
+++ b/INSPIRE/BHR-G INSPIRE mapping.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\brugmanba\OneDrive - TNO\inspire\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vosj1\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="753" documentId="6_{AD577F5D-93E6-4754-B091-D47B7947F923}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{C14FDE00-8F61-4328-A869-E73CF525422C}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8888E422-9381-4AF7-8AF6-774500A9CA1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="versiebeheer" sheetId="5" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="86">
   <si>
     <t>Type</t>
   </si>
@@ -521,13 +521,19 @@
 2) BoreholePurpose versimpeld naar twee waarden, geotechnicalSurvey en geologicalSurvey.
 3) Relatie met GeologicCollection opgenomen (als void)</t>
   </si>
+  <si>
+    <t>Bregje Brugman en Jacob Vos</t>
+  </si>
+  <si>
+    <t>Getoetst met catalogus versie 2.1; geen impact.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="[$-413]d/mmm/yy;@"/>
+    <numFmt numFmtId="164" formatCode="[$-413]d/mmm/yy;@"/>
   </numFmts>
   <fonts count="30" x14ac:knownFonts="1">
     <font>
@@ -1426,57 +1432,84 @@
     <xf numFmtId="0" fontId="21" fillId="35" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="21" fillId="35" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="35" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="34" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="34" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="34" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="37" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="37" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="37" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="37" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="35" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="35" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="35" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="35" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="35" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="35" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="35" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="35" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="35" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="35" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="35" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="35" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="35" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="22" fillId="35" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="35" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="35" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="35" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="35" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="35" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="35" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="35" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="34" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="34" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="34" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="37" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="37" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="22" fillId="33" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="33" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="37" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="37" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="22" fillId="33" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -1488,33 +1521,6 @@
     </xf>
     <xf numFmtId="0" fontId="22" fillId="33" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="35" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="35" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="35" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="35" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="35" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="35" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="35" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="35" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="21" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="62">
@@ -1899,16 +1905,16 @@
   <dimension ref="B2:D15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.7265625" style="1"/>
-    <col min="2" max="2" width="9.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="68.453125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="28.1796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="8.7265625" style="1"/>
+    <col min="1" max="1" width="8.77734375" style="1"/>
+    <col min="2" max="2" width="9.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="68.44140625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="28.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="8.77734375" style="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:4" x14ac:dyDescent="0.25">
@@ -1916,7 +1922,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="3" spans="2:4" ht="29" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:4" ht="28.8" x14ac:dyDescent="0.25">
       <c r="B3" s="16">
         <v>43990</v>
       </c>
@@ -1927,7 +1933,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="4" spans="2:4" ht="72.5" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:4" ht="72" x14ac:dyDescent="0.25">
       <c r="B4" s="16">
         <v>44060</v>
       </c>
@@ -1936,6 +1942,17 @@
       </c>
       <c r="D4" s="1" t="s">
         <v>60</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B5" s="16">
+        <v>44819</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="7" spans="2:4" x14ac:dyDescent="0.25">
@@ -1943,7 +1960,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="8" spans="2:4" ht="101.5" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:4" ht="100.8" x14ac:dyDescent="0.25">
       <c r="B8" s="16">
         <v>44060</v>
       </c>
@@ -1960,7 +1977,7 @@
       </c>
     </row>
     <row r="12" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B12" s="54">
+      <c r="B12" s="40">
         <v>41618</v>
       </c>
       <c r="C12" s="4" t="s">
@@ -1970,8 +1987,8 @@
         <v>71</v>
       </c>
     </row>
-    <row r="13" spans="2:4" ht="29" x14ac:dyDescent="0.25">
-      <c r="B13" s="54" t="s">
+    <row r="13" spans="2:4" ht="28.8" x14ac:dyDescent="0.25">
+      <c r="B13" s="40" t="s">
         <v>82</v>
       </c>
       <c r="C13" s="3" t="s">
@@ -1981,8 +1998,8 @@
         <v>72</v>
       </c>
     </row>
-    <row r="14" spans="2:4" ht="29" x14ac:dyDescent="0.25">
-      <c r="B14" s="54" t="s">
+    <row r="14" spans="2:4" ht="28.8" x14ac:dyDescent="0.25">
+      <c r="B14" s="40" t="s">
         <v>82</v>
       </c>
       <c r="C14" s="3" t="s">
@@ -1993,7 +2010,7 @@
       </c>
     </row>
     <row r="15" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B15" s="54">
+      <c r="B15" s="40">
         <v>43938</v>
       </c>
       <c r="C15" s="3" t="s">
@@ -2013,41 +2030,41 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M34"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="18.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="18.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="4" width="18.54296875" style="6" customWidth="1"/>
-    <col min="5" max="5" width="20.26953125" style="6" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.54296875" style="6" customWidth="1"/>
-    <col min="7" max="7" width="14.26953125" style="6" customWidth="1"/>
-    <col min="8" max="8" width="2.26953125" style="13" customWidth="1"/>
-    <col min="9" max="9" width="20.7265625" style="6" customWidth="1"/>
-    <col min="10" max="10" width="23.81640625" style="6" customWidth="1"/>
-    <col min="11" max="11" width="86.6328125" style="2" customWidth="1"/>
-    <col min="12" max="12" width="71.1796875" style="6" customWidth="1"/>
-    <col min="13" max="16384" width="18.54296875" style="6"/>
+    <col min="1" max="4" width="18.5546875" style="6" customWidth="1"/>
+    <col min="5" max="5" width="20.21875" style="6" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.5546875" style="6" customWidth="1"/>
+    <col min="7" max="7" width="14.21875" style="6" customWidth="1"/>
+    <col min="8" max="8" width="2.21875" style="13" customWidth="1"/>
+    <col min="9" max="9" width="20.77734375" style="6" customWidth="1"/>
+    <col min="10" max="10" width="23.77734375" style="6" customWidth="1"/>
+    <col min="11" max="11" width="86.6640625" style="2" customWidth="1"/>
+    <col min="12" max="12" width="71.21875" style="6" customWidth="1"/>
+    <col min="13" max="16384" width="18.5546875" style="6"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="38" t="s">
+      <c r="A1" s="49" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="39"/>
-      <c r="C1" s="39"/>
-      <c r="D1" s="39"/>
-      <c r="E1" s="39"/>
-      <c r="F1" s="39"/>
-      <c r="G1" s="42"/>
-      <c r="H1" s="40"/>
-      <c r="I1" s="43" t="s">
+      <c r="B1" s="50"/>
+      <c r="C1" s="50"/>
+      <c r="D1" s="50"/>
+      <c r="E1" s="50"/>
+      <c r="F1" s="50"/>
+      <c r="G1" s="51"/>
+      <c r="H1" s="32"/>
+      <c r="I1" s="52" t="s">
         <v>56</v>
       </c>
-      <c r="J1" s="44"/>
-      <c r="K1" s="44"/>
-      <c r="L1" s="45"/>
+      <c r="J1" s="53"/>
+      <c r="K1" s="53"/>
+      <c r="L1" s="54"/>
     </row>
     <row r="2" spans="1:12" ht="66.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
@@ -2068,36 +2085,36 @@
       <c r="F2" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="34" t="s">
+      <c r="G2" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="H2" s="36"/>
-      <c r="I2" s="33" t="s">
+      <c r="H2" s="30"/>
+      <c r="I2" s="27" t="s">
         <v>62</v>
       </c>
       <c r="J2" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="K2" s="35" t="s">
+      <c r="K2" s="29" t="s">
         <v>13</v>
       </c>
       <c r="L2" s="5" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="29" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="52" t="s">
+    <row r="3" spans="1:12" ht="28.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="44" t="s">
         <v>19</v>
       </c>
-      <c r="B3" s="53" t="s">
+      <c r="B3" s="47" t="s">
         <v>20</v>
       </c>
-      <c r="C3" s="47"/>
-      <c r="D3" s="47"/>
-      <c r="E3" s="47"/>
-      <c r="F3" s="47"/>
-      <c r="G3" s="47"/>
-      <c r="H3" s="36"/>
+      <c r="C3" s="35"/>
+      <c r="D3" s="35"/>
+      <c r="E3" s="35"/>
+      <c r="F3" s="35"/>
+      <c r="G3" s="35"/>
+      <c r="H3" s="30"/>
       <c r="I3" s="7" t="s">
         <v>63</v>
       </c>
@@ -2111,9 +2128,9 @@
         <v>55</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="43.5" x14ac:dyDescent="0.25">
-      <c r="A4" s="26"/>
-      <c r="B4" s="27"/>
+    <row r="4" spans="1:12" ht="43.2" x14ac:dyDescent="0.25">
+      <c r="A4" s="45"/>
+      <c r="B4" s="42"/>
       <c r="C4" s="8" t="s">
         <v>6</v>
       </c>
@@ -2129,7 +2146,7 @@
       <c r="G4" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="H4" s="36"/>
+      <c r="H4" s="30"/>
       <c r="I4" s="7" t="s">
         <v>54</v>
       </c>
@@ -2141,9 +2158,9 @@
       </c>
       <c r="L4" s="7"/>
     </row>
-    <row r="5" spans="1:12" ht="43.5" x14ac:dyDescent="0.25">
-      <c r="A5" s="26"/>
-      <c r="B5" s="27"/>
+    <row r="5" spans="1:12" ht="43.2" x14ac:dyDescent="0.25">
+      <c r="A5" s="45"/>
+      <c r="B5" s="42"/>
       <c r="C5" s="8" t="s">
         <v>21</v>
       </c>
@@ -2159,7 +2176,7 @@
       <c r="G5" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="H5" s="36"/>
+      <c r="H5" s="30"/>
       <c r="I5" s="7" t="s">
         <v>54</v>
       </c>
@@ -2173,9 +2190,9 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="29" x14ac:dyDescent="0.25">
-      <c r="A6" s="26"/>
-      <c r="B6" s="27"/>
+    <row r="6" spans="1:12" ht="28.8" x14ac:dyDescent="0.25">
+      <c r="A6" s="45"/>
+      <c r="B6" s="42"/>
       <c r="C6" s="8" t="s">
         <v>24</v>
       </c>
@@ -2191,7 +2208,7 @@
       <c r="G6" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="H6" s="36"/>
+      <c r="H6" s="30"/>
       <c r="I6" s="7" t="s">
         <v>54</v>
       </c>
@@ -2205,9 +2222,9 @@
         <v>38</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="43.5" x14ac:dyDescent="0.25">
-      <c r="A7" s="26"/>
-      <c r="B7" s="27"/>
+    <row r="7" spans="1:12" ht="43.2" x14ac:dyDescent="0.25">
+      <c r="A7" s="45"/>
+      <c r="B7" s="42"/>
       <c r="C7" s="8" t="s">
         <v>26</v>
       </c>
@@ -2223,7 +2240,7 @@
       <c r="G7" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="H7" s="36"/>
+      <c r="H7" s="30"/>
       <c r="I7" s="7" t="s">
         <v>54</v>
       </c>
@@ -2237,9 +2254,9 @@
         <v>61</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="29" x14ac:dyDescent="0.25">
-      <c r="A8" s="26"/>
-      <c r="B8" s="27"/>
+    <row r="8" spans="1:12" ht="28.8" x14ac:dyDescent="0.25">
+      <c r="A8" s="45"/>
+      <c r="B8" s="42"/>
       <c r="C8" s="8" t="s">
         <v>29</v>
       </c>
@@ -2255,7 +2272,7 @@
       <c r="G8" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="H8" s="36"/>
+      <c r="H8" s="30"/>
       <c r="I8" s="7" t="s">
         <v>54</v>
       </c>
@@ -2269,29 +2286,29 @@
         <v>69</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="14.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="26"/>
-      <c r="B9" s="27"/>
-      <c r="C9" s="25" t="s">
+    <row r="9" spans="1:12" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="45"/>
+      <c r="B9" s="42"/>
+      <c r="C9" s="48" t="s">
         <v>9</v>
       </c>
-      <c r="D9" s="28" t="s">
+      <c r="D9" s="41" t="s">
         <v>33</v>
       </c>
-      <c r="E9" s="28" t="s">
+      <c r="E9" s="41" t="s">
         <v>32</v>
       </c>
-      <c r="F9" s="28" t="s">
+      <c r="F9" s="41" t="s">
         <v>8</v>
       </c>
-      <c r="G9" s="28" t="s">
+      <c r="G9" s="41" t="s">
         <v>5</v>
       </c>
-      <c r="H9" s="36"/>
-      <c r="I9" s="51" t="s">
+      <c r="H9" s="30"/>
+      <c r="I9" s="39" t="s">
         <v>54</v>
       </c>
-      <c r="J9" s="30" t="s">
+      <c r="J9" s="25" t="s">
         <v>42</v>
       </c>
       <c r="K9" s="22" t="s">
@@ -2299,17 +2316,17 @@
       </c>
       <c r="L9" s="17"/>
     </row>
-    <row r="10" spans="1:12" ht="87" x14ac:dyDescent="0.25">
-      <c r="A10" s="26"/>
-      <c r="B10" s="27"/>
-      <c r="C10" s="26"/>
-      <c r="D10" s="27"/>
-      <c r="E10" s="27"/>
-      <c r="F10" s="27"/>
-      <c r="G10" s="27"/>
-      <c r="H10" s="36"/>
-      <c r="I10" s="31"/>
-      <c r="J10" s="49"/>
+    <row r="10" spans="1:12" ht="86.4" x14ac:dyDescent="0.25">
+      <c r="A10" s="45"/>
+      <c r="B10" s="42"/>
+      <c r="C10" s="45"/>
+      <c r="D10" s="42"/>
+      <c r="E10" s="42"/>
+      <c r="F10" s="42"/>
+      <c r="G10" s="42"/>
+      <c r="H10" s="30"/>
+      <c r="I10" s="26"/>
+      <c r="J10" s="37"/>
       <c r="K10" s="23" t="s">
         <v>65</v>
       </c>
@@ -2317,17 +2334,17 @@
         <v>66</v>
       </c>
     </row>
-    <row r="11" spans="1:12" ht="29" x14ac:dyDescent="0.25">
-      <c r="A11" s="26"/>
-      <c r="B11" s="27"/>
-      <c r="C11" s="32"/>
-      <c r="D11" s="29"/>
-      <c r="E11" s="29"/>
-      <c r="F11" s="29"/>
-      <c r="G11" s="29"/>
-      <c r="H11" s="36"/>
-      <c r="I11" s="47"/>
-      <c r="J11" s="50"/>
+    <row r="11" spans="1:12" ht="28.8" x14ac:dyDescent="0.25">
+      <c r="A11" s="45"/>
+      <c r="B11" s="42"/>
+      <c r="C11" s="46"/>
+      <c r="D11" s="43"/>
+      <c r="E11" s="43"/>
+      <c r="F11" s="43"/>
+      <c r="G11" s="43"/>
+      <c r="H11" s="30"/>
+      <c r="I11" s="35"/>
+      <c r="J11" s="38"/>
       <c r="K11" s="24" t="s">
         <v>68</v>
       </c>
@@ -2335,9 +2352,9 @@
         <v>67</v>
       </c>
     </row>
-    <row r="12" spans="1:12" s="12" customFormat="1" ht="72.5" x14ac:dyDescent="0.25">
-      <c r="A12" s="32"/>
-      <c r="B12" s="29"/>
+    <row r="12" spans="1:12" s="12" customFormat="1" ht="72" x14ac:dyDescent="0.25">
+      <c r="A12" s="46"/>
+      <c r="B12" s="43"/>
       <c r="C12" s="10" t="s">
         <v>34</v>
       </c>
@@ -2353,7 +2370,7 @@
       <c r="G12" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="H12" s="37"/>
+      <c r="H12" s="31"/>
       <c r="I12" s="7" t="s">
         <v>54</v>
       </c>
@@ -2367,11 +2384,11 @@
         <v>80</v>
       </c>
     </row>
-    <row r="14" spans="1:12" s="12" customFormat="1" ht="58" x14ac:dyDescent="0.25">
-      <c r="A14" s="46" t="s">
+    <row r="14" spans="1:12" s="12" customFormat="1" ht="57.6" x14ac:dyDescent="0.25">
+      <c r="A14" s="34" t="s">
         <v>76</v>
       </c>
-      <c r="B14" s="48" t="s">
+      <c r="B14" s="36" t="s">
         <v>78</v>
       </c>
       <c r="C14" s="10" t="s">
@@ -2389,7 +2406,7 @@
       <c r="G14" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="H14" s="41"/>
+      <c r="H14" s="33"/>
       <c r="I14" s="7" t="s">
         <v>54</v>
       </c>
@@ -2406,21 +2423,23 @@
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="L15" s="2"/>
     </row>
-    <row r="24" spans="12:12" x14ac:dyDescent="0.35">
+    <row r="24" spans="12:12" x14ac:dyDescent="0.3">
       <c r="L24" s="14"/>
     </row>
-    <row r="33" spans="13:13" x14ac:dyDescent="0.35">
+    <row r="33" spans="13:13" x14ac:dyDescent="0.3">
       <c r="M33" s="19" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="34" spans="13:13" x14ac:dyDescent="0.35">
+    <row r="34" spans="13:13" x14ac:dyDescent="0.3">
       <c r="M34" s="20" t="s">
         <v>43</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="I1:L1"/>
     <mergeCell ref="F9:F11"/>
     <mergeCell ref="G9:G11"/>
     <mergeCell ref="A3:A12"/>
@@ -2428,8 +2447,6 @@
     <mergeCell ref="C9:C11"/>
     <mergeCell ref="D9:D11"/>
     <mergeCell ref="E9:E11"/>
-    <mergeCell ref="A1:G1"/>
-    <mergeCell ref="I1:L1"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>